<commit_message>
Plotly feito(sem sistema de peso)
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Documentos\GitHub\Dash-Olimpiadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E1E9EB-9C22-422B-96B6-8417DCC299AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F40B02-96B2-4FD9-BCD2-6C9C33B83BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="2130" windowWidth="20520" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -345,193 +345,193 @@
     <t>Ole Einar Bjørndalen</t>
   </si>
   <si>
-    <t xml:space="preserve"> Bjørn Dæhlie</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Birgit Fischer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sawao Kato</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jenny Thompson</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Matt Biondi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ray Ewry</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nikolay Andrianov</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Boris Shakhlin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Věra Čáslavská</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Viktor Chukarin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aladár Gerevich</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Edoardo Mangiarotti</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marit Bjørgen</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lyubov Egorova</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hubert Van Innis</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Akinori Nakayama</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Valentina Vezzali</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gert Fredriksson</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chris Hoy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vitaly Scherbo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Viktor Ahn</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Reiner Klimke</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pál Kovács</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Usain Bolt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rudolf Kárpáti</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nedo Nadi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kristin Otto</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lidia Skoblikova</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amy Van Dyken</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Takashi Ono</t>
-  </si>
-  <si>
     <t>Carl Osburn</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ryan Lochte</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ágnes Keleti</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nadia Comăneci</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ian Thorpe</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ville Ritola</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Isabell Werth</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Polina Astakhova</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Claudia Pechstein</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elisabeta Lipă</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yukio Endo</t>
-  </si>
-  <si>
     <t>Aaron Peirsol</t>
   </si>
   <si>
-    <t xml:space="preserve"> Mitsuo Tsukahara</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Krisztina Egerszegi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tom Jager</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Larisa Lazutina</t>
-  </si>
-  <si>
-    <t> Michael Phelps</t>
-  </si>
-  <si>
-    <t> Willis Lee</t>
-  </si>
-  <si>
     <t>Clas Thunberg</t>
   </si>
   <si>
-    <t xml:space="preserve"> Hans Günter Winkler</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thomas Alsgaard</t>
-  </si>
-  <si>
     <t>Anton Heida</t>
   </si>
   <si>
-    <t xml:space="preserve"> Nellie Kim</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ole Lilloe-Olsen</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Don Schollander</t>
-  </si>
-  <si>
     <t>Bonnie Blair</t>
   </si>
   <si>
-    <t xml:space="preserve"> Georgeta Damian</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alfred Lane</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Steve Redgrave</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Johnny Weissmuller</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Morris Fisher</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eric Heiden</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gary Hall Jr.</t>
+    <t>Michael Phelps</t>
+  </si>
+  <si>
+    <t>Bjørn Dæhlie</t>
+  </si>
+  <si>
+    <t>Birgit Fischer</t>
+  </si>
+  <si>
+    <t>Sawao Kato</t>
+  </si>
+  <si>
+    <t>Jenny Thompson</t>
+  </si>
+  <si>
+    <t>Matt Biondi</t>
+  </si>
+  <si>
+    <t>Ray Ewry</t>
+  </si>
+  <si>
+    <t>Boris Shakhlin</t>
+  </si>
+  <si>
+    <t>Nikolay Andrianov</t>
+  </si>
+  <si>
+    <t>Věra Čáslavská</t>
+  </si>
+  <si>
+    <t>Viktor Chukarin</t>
+  </si>
+  <si>
+    <t>Aladár Gerevich</t>
+  </si>
+  <si>
+    <t>Edoardo Mangiarotti</t>
+  </si>
+  <si>
+    <t>Valentina Vezzali</t>
+  </si>
+  <si>
+    <t>Akinori Nakayama</t>
+  </si>
+  <si>
+    <t>Lyubov Egorova</t>
+  </si>
+  <si>
+    <t>Hubert Van Innis</t>
+  </si>
+  <si>
+    <t>Marit Bjørgen</t>
+  </si>
+  <si>
+    <t>Gert Fredriksson</t>
+  </si>
+  <si>
+    <t>Chris Hoy</t>
+  </si>
+  <si>
+    <t>Vitaly Scherbo</t>
+  </si>
+  <si>
+    <t>Viktor Ahn</t>
+  </si>
+  <si>
+    <t>Reiner Klimke</t>
+  </si>
+  <si>
+    <t>Pál Kovács</t>
+  </si>
+  <si>
+    <t>Usain Bolt</t>
+  </si>
+  <si>
+    <t>Rudolf Kárpáti</t>
+  </si>
+  <si>
+    <t>Nedo Nadi</t>
+  </si>
+  <si>
+    <t>Kristin Otto</t>
+  </si>
+  <si>
+    <t>Lidia Skoblikova</t>
+  </si>
+  <si>
+    <t>Amy Van Dyken</t>
+  </si>
+  <si>
+    <t>Takashi Ono</t>
+  </si>
+  <si>
+    <t>Ryan Lochte</t>
+  </si>
+  <si>
+    <t>Gary Hall Jr.</t>
+  </si>
+  <si>
+    <t>Ágnes Keleti</t>
+  </si>
+  <si>
+    <t>Nadia Comăneci</t>
+  </si>
+  <si>
+    <t>Ian Thorpe</t>
+  </si>
+  <si>
+    <t>Ville Ritola</t>
+  </si>
+  <si>
+    <t>Isabell Werth</t>
+  </si>
+  <si>
+    <t>Polina Astakhova</t>
+  </si>
+  <si>
+    <t>Claudia Pechstein</t>
+  </si>
+  <si>
+    <t>Elisabeta Lipă</t>
+  </si>
+  <si>
+    <t>Yukio Endo</t>
+  </si>
+  <si>
+    <t>Mitsuo Tsukahara</t>
+  </si>
+  <si>
+    <t>Krisztina Egerszegi</t>
+  </si>
+  <si>
+    <t>Tom Jager</t>
+  </si>
+  <si>
+    <t>Larisa Lazutina</t>
+  </si>
+  <si>
+    <t>Willis Lee</t>
+  </si>
+  <si>
+    <t>Hans Günter Winkler</t>
+  </si>
+  <si>
+    <t>Thomas Alsgaard</t>
+  </si>
+  <si>
+    <t>Nellie Kim</t>
+  </si>
+  <si>
+    <t>Ole Lilloe-Olsen</t>
+  </si>
+  <si>
+    <t>Don Schollander</t>
+  </si>
+  <si>
+    <t>Georgeta Damian</t>
+  </si>
+  <si>
+    <t>Alfred Lane</t>
+  </si>
+  <si>
+    <t>Steve Redgrave</t>
+  </si>
+  <si>
+    <t>Johnny Weissmuller</t>
+  </si>
+  <si>
+    <t>Morris Fisher</t>
+  </si>
+  <si>
+    <t>Eric Heiden</t>
   </si>
 </sst>
 </file>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>11</v>
@@ -1216,7 +1216,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>25</v>
@@ -1251,7 +1251,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>31</v>
@@ -1286,7 +1286,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>34</v>
@@ -1321,7 +1321,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>11</v>
@@ -1356,7 +1356,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>11</v>
@@ -1391,7 +1391,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>11</v>
@@ -1426,7 +1426,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>16</v>
@@ -1461,7 +1461,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>16</v>
@@ -1496,7 +1496,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>40</v>
@@ -1531,7 +1531,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>16</v>
@@ -1566,7 +1566,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>43</v>
@@ -1601,7 +1601,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>46</v>
@@ -1636,7 +1636,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>25</v>
@@ -1671,7 +1671,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>49</v>
@@ -1706,7 +1706,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>51</v>
@@ -1741,7 +1741,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>34</v>
@@ -1776,7 +1776,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>46</v>
@@ -1811,7 +1811,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>56</v>
@@ -1846,7 +1846,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>58</v>
@@ -1881,7 +1881,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>61</v>
@@ -1916,7 +1916,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>63</v>
@@ -1949,7 +1949,7 @@
     <row r="29" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="5" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>31</v>
@@ -1984,7 +1984,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>43</v>
@@ -2019,7 +2019,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>68</v>
@@ -2054,7 +2054,7 @@
         <v>18</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>43</v>
@@ -2089,7 +2089,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>46</v>
@@ -2124,7 +2124,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>71</v>
@@ -2159,7 +2159,7 @@
         <v>30</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>16</v>
@@ -2194,7 +2194,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>11</v>
@@ -2229,7 +2229,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>34</v>
@@ -2264,7 +2264,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>11</v>
@@ -2299,7 +2299,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>11</v>
@@ -2334,7 +2334,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>11</v>
@@ -2369,7 +2369,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>43</v>
@@ -2404,7 +2404,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>80</v>
@@ -2439,7 +2439,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>82</v>
@@ -2474,7 +2474,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>20</v>
@@ -2509,7 +2509,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>31</v>
@@ -2544,7 +2544,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>16</v>
@@ -2579,7 +2579,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>31</v>
@@ -2614,7 +2614,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>80</v>
@@ -2649,7 +2649,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>34</v>
@@ -2684,7 +2684,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>11</v>
@@ -2719,7 +2719,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>34</v>
@@ -2754,7 +2754,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>43</v>
@@ -2789,7 +2789,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>11</v>
@@ -2824,7 +2824,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>49</v>
@@ -2859,7 +2859,7 @@
         <v>51</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>11</v>
@@ -2894,7 +2894,7 @@
         <v>51</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>20</v>
@@ -2924,12 +2924,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>51</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>31</v>
@@ -2964,7 +2964,7 @@
         <v>51</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>25</v>
@@ -2999,7 +2999,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>11</v>
@@ -3034,7 +3034,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>16</v>
@@ -3069,7 +3069,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>25</v>
@@ -3104,7 +3104,7 @@
         <v>57</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>11</v>
@@ -3139,7 +3139,7 @@
         <v>57</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>160</v>
+        <v>109</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>11</v>
@@ -3174,7 +3174,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>80</v>
@@ -3209,7 +3209,7 @@
         <v>62</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>11</v>
@@ -3244,7 +3244,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>58</v>
@@ -3279,7 +3279,7 @@
         <v>62</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>11</v>
@@ -3349,7 +3349,7 @@
         <v>62</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>11</v>
@@ -3384,7 +3384,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>11</v>

</xml_diff>